<commit_message>
Update Juptyer + filled in new excel
</commit_message>
<xml_diff>
--- a/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
+++ b/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032B6437-982C-43DF-BDCB-FE18EEDBECCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95559B6-3CA2-4E84-80A9-04438A059760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2280" yWindow="-18930" windowWidth="28800" windowHeight="15225" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-28920" yWindow="-5475" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
+    <sheet name="Storage" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
   <si>
     <t>Unit</t>
   </si>
@@ -83,18 +84,9 @@
     <t>Cost_var</t>
   </si>
   <si>
-    <t>Capacity_existing</t>
-  </si>
-  <si>
-    <t>Capacity_max</t>
-  </si>
-  <si>
     <t>CO2_Vaporizer</t>
   </si>
   <si>
-    <t>Corbon_Dioxide</t>
-  </si>
-  <si>
     <t>Vaporized_Carbon_Dioxide</t>
   </si>
   <si>
@@ -105,16 +97,100 @@
   </si>
   <si>
     <t>Raw_Methanol</t>
+  </si>
+  <si>
+    <t>Destilation_Tower</t>
+  </si>
+  <si>
+    <t>power_line_Wholesale_Kasso</t>
+  </si>
+  <si>
+    <t>Power_Wholesale</t>
+  </si>
+  <si>
+    <t>Power_Kasso</t>
+  </si>
+  <si>
+    <t>pipeline_storage_hydrogen</t>
+  </si>
+  <si>
+    <t>pipeline_storage_e-methanol</t>
+  </si>
+  <si>
+    <t>pipeline_District_Heating</t>
+  </si>
+  <si>
+    <t>Hydrogen_storage_Kasso</t>
+  </si>
+  <si>
+    <t>E-methanol_Kasso</t>
+  </si>
+  <si>
+    <t>E-methanol_storage_Kasso</t>
+  </si>
+  <si>
+    <t>Waste_Heat</t>
+  </si>
+  <si>
+    <t>E-Methanol_storage_Kasso</t>
+  </si>
+  <si>
+    <t>E-Methanol_Kasso</t>
+  </si>
+  <si>
+    <t>District_Heating</t>
+  </si>
+  <si>
+    <t>Solar_Plant_Kasso</t>
+  </si>
+  <si>
+    <t>Carbon_Dioxide</t>
+  </si>
+  <si>
+    <t>Cap_Input1_existing</t>
+  </si>
+  <si>
+    <t>Cap_Input2_max</t>
+  </si>
+  <si>
+    <t>Cap_Input1_max</t>
+  </si>
+  <si>
+    <t>Cap_Input2_existing</t>
+  </si>
+  <si>
+    <t>Cap_Output1_max</t>
+  </si>
+  <si>
+    <t>Cap_Output1_existing</t>
+  </si>
+  <si>
+    <t>Cap_Output2_existing</t>
+  </si>
+  <si>
+    <t>Cap_Output2_max</t>
+  </si>
+  <si>
+    <t>Cap_Output_1_max</t>
+  </si>
+  <si>
+    <t>Connection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -160,22 +236,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:M4" totalsRowShown="0">
-  <autoFilter ref="A1:M4" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:S6" totalsRowShown="0">
+  <autoFilter ref="A1:S6" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{C03E717E-B39B-450F-A07B-8C087AA65297}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{1193D369-BC65-45A6-8749-4CD88E2C1722}" name="Output2"/>
-    <tableColumn id="6" xr3:uid="{4AAC878F-692F-4277-A013-661DCC5DAE26}" name="Capacity_existing"/>
-    <tableColumn id="7" xr3:uid="{C21757F9-61E8-45D7-ADA3-80D8624CAEF0}" name="Capacity_max"/>
+    <tableColumn id="6" xr3:uid="{4AAC878F-692F-4277-A013-661DCC5DAE26}" name="Cap_Input1_existing"/>
+    <tableColumn id="7" xr3:uid="{C21757F9-61E8-45D7-ADA3-80D8624CAEF0}" name="Cap_Input1_max"/>
+    <tableColumn id="14" xr3:uid="{23796EE3-B67D-45AE-9553-CC3081EFDF57}" name="Cap_Input2_existing"/>
+    <tableColumn id="15" xr3:uid="{DF0C0799-CA68-4E9B-A1FB-41F4996C01A9}" name="Cap_Input2_max"/>
+    <tableColumn id="16" xr3:uid="{8A84DF9A-0F8E-4DA8-A009-F41EF2B05A60}" name="Cap_Output1_existing"/>
+    <tableColumn id="17" xr3:uid="{6408F114-841E-472E-92F5-7B63FF1B66F4}" name="Cap_Output_1_max"/>
+    <tableColumn id="18" xr3:uid="{541C17F0-C020-47FE-9DA4-DB76D7416668}" name="Cap_Output2_existing"/>
+    <tableColumn id="19" xr3:uid="{D6FEE63D-DC89-4D1A-9708-5E7C70FD5793}" name="Cap_Output2_max"/>
     <tableColumn id="8" xr3:uid="{5F719CEE-A0F7-452C-B82C-E739C5FED49B}" name="Efficency"/>
     <tableColumn id="9" xr3:uid="{50F936EF-D32C-4938-8FCA-291A6A3E82E6}" name="Relation_Input"/>
     <tableColumn id="10" xr3:uid="{ACDE4024-BCA2-4145-B3BC-1A5A08F3EA7D}" name="Relation_Output"/>
     <tableColumn id="11" xr3:uid="{8AEC88A1-B64A-43A2-AC89-3B27AB4ACAD7}" name="Cost_invest"/>
     <tableColumn id="12" xr3:uid="{F1A83AF0-CF23-4B00-9076-4E28DF8DAFD3}" name="Cost_OM"/>
     <tableColumn id="13" xr3:uid="{AD4231E3-CB94-4597-81A2-E13C044BBD2D}" name="Cost_var"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{856854C3-DC05-4AB8-91B8-0E52D9C11DBC}" name="Table13" displayName="Table13" ref="A1:S5" totalsRowShown="0">
+  <autoFilter ref="A1:S5" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{26B0CA71-1EA9-44CF-8E6D-31054ECA99A6}" name="Connection"/>
+    <tableColumn id="2" xr3:uid="{587ADBB8-7B68-42BE-A14F-535C6116E5EA}" name="Input1"/>
+    <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
+    <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
+    <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output2"/>
+    <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Cap_Input1_existing"/>
+    <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_max"/>
+    <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input2_existing"/>
+    <tableColumn id="7" xr3:uid="{E7E4A800-7F3E-4BF9-A884-F3BDD87E4621}" name="Cap_Input2_max"/>
+    <tableColumn id="16" xr3:uid="{8893BE03-F801-4096-BA71-49D3B6176542}" name="Cap_Output1_existing"/>
+    <tableColumn id="17" xr3:uid="{9DC965EA-6654-4828-B29B-097368A09D75}" name="Cap_Output1_max"/>
+    <tableColumn id="19" xr3:uid="{CB576510-488A-48D1-9EBF-E417CAAAB7E4}" name="Cap_Output2_existing"/>
+    <tableColumn id="20" xr3:uid="{5176DB25-AD8B-43E3-AEAF-7F27C99BEFB0}" name="Cap_Output2_max"/>
+    <tableColumn id="8" xr3:uid="{5E25F56C-3E8C-4A4F-ACEB-CDBC45CA165F}" name="Efficency"/>
+    <tableColumn id="9" xr3:uid="{3138804A-F699-4287-89C7-DE76BAD06195}" name="Relation_Input"/>
+    <tableColumn id="10" xr3:uid="{AE158189-8F74-4D1A-BE7F-20B56DC1FCA0}" name="Relation_Output"/>
+    <tableColumn id="11" xr3:uid="{ADDA3F91-13EA-44FD-BDAD-129E45FF1B77}" name="Cost_invest"/>
+    <tableColumn id="12" xr3:uid="{19693C8E-93B1-45BA-838A-11FFE3971C45}" name="Cost_OM"/>
+    <tableColumn id="13" xr3:uid="{9A50D747-7636-48C7-AEA4-AC76517E91C7}" name="Cost_var"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -478,27 +588,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.81640625" customWidth="1"/>
     <col min="4" max="5" width="9.81640625" customWidth="1"/>
-    <col min="6" max="6" width="17.6328125" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" customWidth="1"/>
-    <col min="8" max="8" width="10.54296875" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" customWidth="1"/>
-    <col min="10" max="10" width="16.90625" customWidth="1"/>
-    <col min="11" max="11" width="12.7265625" customWidth="1"/>
-    <col min="12" max="12" width="10.6328125" customWidth="1"/>
-    <col min="13" max="13" width="10.08984375" customWidth="1"/>
+    <col min="6" max="6" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" customWidth="1"/>
+    <col min="15" max="15" width="15.453125" customWidth="1"/>
+    <col min="16" max="16" width="16.90625" customWidth="1"/>
+    <col min="17" max="17" width="12.7265625" customWidth="1"/>
+    <col min="18" max="18" width="10.6328125" customWidth="1"/>
+    <col min="19" max="19" width="10.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,100 +631,398 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>304</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>52</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>100</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
+  <dimension ref="A1:S5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="4" max="5" width="9.81640625" customWidth="1"/>
+    <col min="6" max="6" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.36328125" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" customWidth="1"/>
+    <col min="15" max="15" width="15.453125" customWidth="1"/>
+    <col min="16" max="16" width="16.90625" customWidth="1"/>
+    <col min="17" max="17" width="12.7265625" customWidth="1"/>
+    <col min="18" max="18" width="10.6328125" customWidth="1"/>
+    <col min="19" max="19" width="10.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1000</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="L2">
         <v>1</v>
       </c>
       <c r="M2">
+        <v>1000</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
+      <c r="I3">
+        <v>1000</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>1000</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1000</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
first step of update input sheet generation
</commit_message>
<xml_diff>
--- a/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
+++ b/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A053AED-A777-4188-9976-770F7AAE962F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88600A81-37D2-414D-B427-B21824A89A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-5475" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Node_slack_penalties are not working yet
Everything else should be included except for the node_slack_penalties, which contain some sort of error
</commit_message>
<xml_diff>
--- a/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
+++ b/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1F0FDE-714F-4041-907A-DD83D4CF0E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291BC95A-EA5B-4652-A08A-362F8E0390B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>Unit</t>
   </si>
@@ -172,13 +172,37 @@
     <t>Storage</t>
   </si>
   <si>
-    <t>has_stae</t>
-  </si>
-  <si>
-    <t>xy</t>
-  </si>
-  <si>
-    <t>type</t>
+    <t>Connection_type</t>
+  </si>
+  <si>
+    <t>connection_type_lossless_bidirectional</t>
+  </si>
+  <si>
+    <t>connection_type_normal</t>
+  </si>
+  <si>
+    <t>has_state</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>node_state_cap</t>
+  </si>
+  <si>
+    <t>frac_state_loss</t>
+  </si>
+  <si>
+    <t>node_state</t>
+  </si>
+  <si>
+    <t>value_before</t>
+  </si>
+  <si>
+    <t>value_start</t>
+  </si>
+  <si>
+    <t>fix_node_state</t>
   </si>
 </sst>
 </file>
@@ -220,13 +244,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -269,14 +306,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{856854C3-DC05-4AB8-91B8-0E52D9C11DBC}" name="Table13" displayName="Table13" ref="A1:U5" totalsRowShown="0">
-  <autoFilter ref="A1:U5" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{856854C3-DC05-4AB8-91B8-0E52D9C11DBC}" name="Table13" displayName="Table13" ref="A1:V5" totalsRowShown="0">
+  <autoFilter ref="A1:V5" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{26B0CA71-1EA9-44CF-8E6D-31054ECA99A6}" name="Connection"/>
     <tableColumn id="2" xr3:uid="{587ADBB8-7B68-42BE-A14F-535C6116E5EA}" name="Input1"/>
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output2"/>
+    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Cap_Input1_existing"/>
     <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_max"/>
     <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input2_existing"/>
@@ -289,36 +327,28 @@
     <tableColumn id="18" xr3:uid="{5D07405F-AE18-4D9F-96A6-B56AE42485A2}" name="Relation_In_In"/>
     <tableColumn id="9" xr3:uid="{3138804A-F699-4287-89C7-DE76BAD06195}" name="Relation_In_Out"/>
     <tableColumn id="10" xr3:uid="{AE158189-8F74-4D1A-BE7F-20B56DC1FCA0}" name="Relation_Out_Out"/>
+    <tableColumn id="23" xr3:uid="{C3B5D3DD-6B9E-4750-8098-2BDCA6D4F76B}" name="Column1"/>
     <tableColumn id="11" xr3:uid="{ADDA3F91-13EA-44FD-BDAD-129E45FF1B77}" name="Cost_invest"/>
     <tableColumn id="12" xr3:uid="{19693C8E-93B1-45BA-838A-11FFE3971C45}" name="Cost_OM"/>
     <tableColumn id="13" xr3:uid="{9A50D747-7636-48C7-AEA4-AC76517E91C7}" name="Cost_var"/>
-    <tableColumn id="21" xr3:uid="{A93B9560-4F92-440E-BD2C-53E892172570}" name="type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:T5" totalsRowShown="0">
-  <autoFilter ref="A1:T5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
-  <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage"/>
-    <tableColumn id="2" xr3:uid="{0A3ACDAB-3D39-4FB6-A742-B7CBC1FE00D3}" name="Input1"/>
-    <tableColumn id="3" xr3:uid="{9CF46F40-4D8F-4B79-9E1F-90679F8E52BE}" name="Input2"/>
-    <tableColumn id="4" xr3:uid="{B8D7EF1E-B2F7-4306-B91F-22F69E6F5B6D}" name="Output1"/>
-    <tableColumn id="5" xr3:uid="{58DBFD58-A0D2-4B31-B639-19B1628ABAC8}" name="has_stae"/>
-    <tableColumn id="6" xr3:uid="{C94AD97A-09DA-4F17-9C68-FBD33CC87E31}" name="Cap_Input1_existing"/>
-    <tableColumn id="15" xr3:uid="{FF9276D0-2590-473A-9C61-1D50612CE008}" name="Cap_Input1_max"/>
-    <tableColumn id="14" xr3:uid="{CFEE349B-BE32-44A5-98DD-3F11A7297C0D}" name="Cap_Input2_existing"/>
-    <tableColumn id="7" xr3:uid="{EB5AE939-F93F-4897-AAEF-1C3F93D54696}" name="Cap_Input2_max"/>
-    <tableColumn id="16" xr3:uid="{A0D87768-BAF8-4A8A-9F7B-A7BAB439FB91}" name="Cap_Output1_existing"/>
-    <tableColumn id="17" xr3:uid="{4243D56B-A005-48D7-90E7-C142DC3460F5}" name="Cap_Output1_max"/>
-    <tableColumn id="19" xr3:uid="{6C11441D-043B-49DF-8662-BCB9AF565AD2}" name="Cap_Output2_existing"/>
-    <tableColumn id="20" xr3:uid="{A1099428-5C48-4F6C-8F48-F3F72DAF5B10}" name="Cap_Output2_max"/>
-    <tableColumn id="8" xr3:uid="{39BA73B9-211C-4B8F-8C41-4B9904C3BAD6}" name="Efficency"/>
-    <tableColumn id="18" xr3:uid="{A4FD28BB-DABC-402E-A908-C27AE58A6ECC}" name="Relation_In_In"/>
-    <tableColumn id="9" xr3:uid="{E42D5CDA-7722-4EBE-9BC9-AA68E17EE52B}" name="Relation_In_Out"/>
-    <tableColumn id="10" xr3:uid="{8B80CBF5-0728-441D-AB6B-6D441D20F584}" name="Relation_Out_Out"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:J5" totalsRowShown="0">
+  <autoFilter ref="A1:J5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="1">
+      <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{AEAA1B51-84C1-491F-81D5-7757B30BDCCD}" name="value_before"/>
+    <tableColumn id="6" xr3:uid="{FA5F8582-61FC-4A96-9E8D-E08E92F1962D}" name="value_start"/>
+    <tableColumn id="5" xr3:uid="{58DBFD58-A0D2-4B31-B639-19B1628ABAC8}" name="has_state"/>
+    <tableColumn id="2" xr3:uid="{1FB70133-79C8-41A8-BCD5-AC8AA5856E5B}" name="node_state_cap"/>
+    <tableColumn id="3" xr3:uid="{11AD2EA9-CE36-4CCE-8F89-387EFE0D8EED}" name="frac_state_loss"/>
+    <tableColumn id="7" xr3:uid="{FDFFF561-E931-46C6-8D90-30C5BF9CB9E9}" name="node_state"/>
     <tableColumn id="11" xr3:uid="{3C880482-B284-4120-859D-C69724716B06}" name="Cost_invest"/>
     <tableColumn id="12" xr3:uid="{DC155748-1945-4E24-B8A1-527B52E12445}" name="Cost_OM"/>
     <tableColumn id="13" xr3:uid="{620A5657-4B04-4066-87F7-215E607C4C88}" name="Cost_var"/>
@@ -627,7 +657,7 @@
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -839,34 +869,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.81640625" customWidth="1"/>
     <col min="4" max="5" width="9.81640625" customWidth="1"/>
-    <col min="6" max="6" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="20.36328125" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.54296875" customWidth="1"/>
-    <col min="15" max="15" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7265625" customWidth="1"/>
-    <col min="19" max="19" width="10.6328125" customWidth="1"/>
-    <col min="20" max="20" width="10.08984375" customWidth="1"/>
+    <col min="6" max="6" width="17.08984375" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="15.36328125" customWidth="1"/>
+    <col min="10" max="10" width="1.7265625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="15.36328125" customWidth="1"/>
+    <col min="12" max="12" width="19" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="15.36328125" customWidth="1"/>
+    <col min="14" max="14" width="19" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="10.54296875" customWidth="1"/>
+    <col min="16" max="16" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.81640625" customWidth="1"/>
+    <col min="20" max="20" width="12.7265625" customWidth="1"/>
+    <col min="21" max="21" width="10.6328125" customWidth="1"/>
+    <col min="22" max="22" width="10.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -883,55 +915,58 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>34</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>36</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>41</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>42</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T1" t="s">
         <v>8</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>9</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>10</v>
       </c>
-      <c r="U1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -947,8 +982,8 @@
       <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="F2">
-        <v>1000</v>
+      <c r="F2" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="G2">
         <v>1000</v>
@@ -971,8 +1006,11 @@
       <c r="M2">
         <v>1000</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="N2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -988,8 +1026,8 @@
       <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="H3">
-        <v>1000</v>
+      <c r="F3" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="I3">
         <v>1000</v>
@@ -1000,11 +1038,14 @@
       <c r="K3">
         <v>1000</v>
       </c>
-      <c r="P3">
+      <c r="L3">
+        <v>1000</v>
+      </c>
+      <c r="Q3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1020,8 +1061,8 @@
       <c r="E4" t="s">
         <v>26</v>
       </c>
-      <c r="H4">
-        <v>1000</v>
+      <c r="F4" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="I4">
         <v>1000</v>
@@ -1032,8 +1073,11 @@
       <c r="K4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1043,16 +1087,19 @@
       <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="F5">
-        <v>1000</v>
+      <c r="F5" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="G5">
         <v>1000</v>
       </c>
-      <c r="J5">
+      <c r="H5">
         <v>1000</v>
       </c>
       <c r="K5">
+        <v>1000</v>
+      </c>
+      <c r="L5">
         <v>1000</v>
       </c>
     </row>
@@ -1067,85 +1114,100 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" t="s">
-        <v>32</v>
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" t="s">
-        <v>8</v>
-      </c>
-      <c r="S1" t="s">
-        <v>9</v>
-      </c>
-      <c r="T1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>100000</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>100000</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
include connection information into the slack penalty input creation
</commit_message>
<xml_diff>
--- a/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
+++ b/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291BC95A-EA5B-4652-A08A-362F8E0390B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7FA07C-C751-421F-AB85-252BCEB41EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -244,14 +244,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -259,9 +261,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -314,7 +313,7 @@
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input2"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Output1"/>
     <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output2"/>
-    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="0"/>
+    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Connection_type" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Cap_Input1_existing"/>
     <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_max"/>
     <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input2_existing"/>
@@ -340,7 +339,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:J5" totalsRowShown="0">
   <autoFilter ref="A1:J5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0">
       <calculatedColumnFormula array="1">_xlfn._xlws.FILTER(Connections!A2:A100,ISNUMBER(FIND("storage",Connections!A2:A100)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{AEAA1B51-84C1-491F-81D5-7757B30BDCCD}" name="value_before"/>
@@ -872,7 +871,7 @@
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -982,7 +981,7 @@
       <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>45</v>
       </c>
       <c r="G2">
@@ -1026,7 +1025,7 @@
       <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>45</v>
       </c>
       <c r="I3">
@@ -1061,7 +1060,7 @@
       <c r="E4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>45</v>
       </c>
       <c r="I4">
@@ -1087,7 +1086,7 @@
       <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>46</v>
       </c>
       <c r="G5">
@@ -1147,13 +1146,13 @@
       <c r="D1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>51</v>
       </c>
       <c r="H1" t="s">

</xml_diff>

<commit_message>
Added missing Output in Excel Database
</commit_message>
<xml_diff>
--- a/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
+++ b/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanaJosephineHentsch\OneDrive - CBS - Copenhagen Business School\Dokumente\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9A2B61-5FDA-477F-A17D-22BADCC66372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CEF41D-1762-4B71-9DF2-19905F732645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-28920" yWindow="-3165" windowWidth="29040" windowHeight="15720" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
   <si>
     <t>Unit</t>
   </si>
@@ -656,7 +656,7 @@
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -809,6 +809,9 @@
       <c r="B5" t="s">
         <v>15</v>
       </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
       <c r="F5">
         <v>52</v>
       </c>
@@ -871,7 +874,7 @@
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added another source of district_heating
used to only be generated from the electrolyzer, now it is also generated by the methanol reactor
</commit_message>
<xml_diff>
--- a/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
+++ b/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanaJosephineHentsch\OneDrive - CBS - Copenhagen Business School\Dokumente\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CEF41D-1762-4B71-9DF2-19905F732645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B088AF04-368C-47E6-BED8-ED7C3E5764B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3165" windowWidth="29040" windowHeight="15720" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -800,6 +800,9 @@
       </c>
       <c r="P4">
         <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Revert "Added another source of district_heating"
This reverts commit 8340ca59d4b95d30901f7a7128984df6f5bc1b59.
</commit_message>
<xml_diff>
--- a/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
+++ b/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanaJosephineHentsch\OneDrive - CBS - Copenhagen Business School\Dokumente\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B088AF04-368C-47E6-BED8-ED7C3E5764B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CEF41D-1762-4B71-9DF2-19905F732645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-28920" yWindow="-3165" windowWidth="29040" windowHeight="15720" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -800,9 +800,6 @@
       </c>
       <c r="P4">
         <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added additional source of district_heat
Also changed the ratio of heat generation to 20 each instead of 4 (which was arbitrary anyways)
</commit_message>
<xml_diff>
--- a/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
+++ b/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanaJosephineHentsch\OneDrive - CBS - Copenhagen Business School\Dokumente\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djh.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2CEF41D-1762-4B71-9DF2-19905F732645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5F129C-F796-4163-9AFB-C70E6C3320D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3165" windowWidth="29040" windowHeight="15720" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -781,6 +781,9 @@
       <c r="P3">
         <v>2</v>
       </c>
+      <c r="Q3">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -857,7 +860,7 @@
         <v>1</v>
       </c>
       <c r="Q6">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug on balance_type creation
bug causes infeasible problems as source nodes must be balanced currently
</commit_message>
<xml_diff>
--- a/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
+++ b/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F87E9F7-2F23-43A3-B88D-43F78273FCD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CFCF78-59AF-403D-931C-867961C45B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
   <si>
     <t>Unit</t>
   </si>
@@ -176,9 +176,6 @@
   </si>
   <si>
     <t>connection_type_lossless_bidirectional</t>
-  </si>
-  <si>
-    <t>connection_type_normal</t>
   </si>
   <si>
     <t>has_state</t>
@@ -877,7 +874,7 @@
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -959,7 +956,7 @@
         <v>42</v>
       </c>
       <c r="S1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T1" t="s">
         <v>8</v>
@@ -1089,11 +1086,17 @@
       <c r="B5" t="s">
         <v>24</v>
       </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
       <c r="D5" t="s">
         <v>27</v>
       </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5">
         <v>1000</v>
@@ -1144,22 +1147,22 @@
         <v>43</v>
       </c>
       <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
-        <v>53</v>
-      </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>50</v>
-      </c>
-      <c r="G1" t="s">
-        <v>51</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -1188,7 +1191,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -1208,7 +1211,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hot fix balance type node creation
automation of balance type creation is not working properly
</commit_message>
<xml_diff>
--- a/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
+++ b/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CFCF78-59AF-403D-931C-867961C45B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD564A63-4303-4B4A-A658-F8C42A7A230D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -793,7 +793,7 @@
         <v>12</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="K4">
         <v>100</v>
@@ -812,10 +812,10 @@
       <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>52</v>
       </c>
-      <c r="G5">
+      <c r="J5">
         <v>52</v>
       </c>
       <c r="P5">
@@ -839,13 +839,13 @@
         <v>24</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="K6">
         <v>100</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="M6">
         <v>10</v>
@@ -874,7 +874,7 @@
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1104,10 +1104,16 @@
       <c r="H5">
         <v>1000</v>
       </c>
+      <c r="I5">
+        <v>1000</v>
+      </c>
       <c r="K5">
         <v>1000</v>
       </c>
       <c r="L5">
+        <v>1000</v>
+      </c>
+      <c r="M5">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix relation flow bug
</commit_message>
<xml_diff>
--- a/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
+++ b/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD564A63-4303-4B4A-A658-F8C42A7A230D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27219837-737D-418B-81A5-4C3ED14D4290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -652,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -775,11 +775,8 @@
       <c r="G3">
         <v>52</v>
       </c>
-      <c r="P3">
+      <c r="O3">
         <v>2</v>
-      </c>
-      <c r="Q3">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
@@ -857,7 +854,7 @@
         <v>1</v>
       </c>
       <c r="Q6">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -873,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
update data prep + model run
</commit_message>
<xml_diff>
--- a/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
+++ b/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFCD4332-A553-4A60-8531-5AB3D3316C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0526DEF4-9719-470D-8B83-EE2779E26E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
   <si>
     <t>Unit</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t>Relation_Out_In</t>
+  </si>
+  <si>
+    <t>connection_type_normal</t>
   </si>
 </sst>
 </file>
@@ -652,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -870,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z20" sqref="Z20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1089,17 +1092,11 @@
       <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
       <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="G5">
         <v>1000</v>
@@ -1107,16 +1104,10 @@
       <c r="H5">
         <v>1000</v>
       </c>
-      <c r="I5">
-        <v>1000</v>
-      </c>
       <c r="K5">
         <v>1000</v>
       </c>
       <c r="L5">
-        <v>1000</v>
-      </c>
-      <c r="M5">
         <v>1000</v>
       </c>
       <c r="S5">

</xml_diff>

<commit_message>
test run with new eff inputs
</commit_message>
<xml_diff>
--- a/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
+++ b/Spine_Projects/Input_data/Input_raw/Model_Data_Base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\Spine_Projects\Input_data\Input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3B0E36-7C8B-4C2A-9E66-07C5C038A4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3853F5-0F8A-4751-B92B-6D63D45C6909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="1020" yWindow="-18540" windowWidth="28800" windowHeight="15225" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -779,7 +779,7 @@
         <v>52</v>
       </c>
       <c r="O3">
-        <v>2</v>
+        <v>4.7614285714285716</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>